<commit_message>
Updated BOM with received items
</commit_message>
<xml_diff>
--- a/doc/BOM.xlsx
+++ b/doc/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Documents\02_ETSII\1MII\2\DASE\Regulator\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9077517F-DF6F-4363-83B4-2AC935EDA7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DCC1BD-5B7A-446D-A5AE-9635E2153048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6D133A79-9F30-48DA-A208-1AC2C38546E4}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="36" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="71">
   <si>
     <t>--- Bill of Materials ---</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>TO222 Heatsink*</t>
+  </si>
+  <si>
+    <t>Obtenido</t>
   </si>
 </sst>
 </file>
@@ -352,21 +355,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -376,17 +379,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -619,7 +635,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D7094093-D7AC-4CE4-AC9B-10203550868F}" name="PivotTable2" cacheId="36" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D7094093-D7AC-4CE4-AC9B-10203550868F}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:O9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" showAll="0"/>
@@ -1557,7 +1573,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="123" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1634,38 +1650,34 @@
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>2</v>
       </c>
-      <c r="I3" s="3">
-        <v>1</v>
-      </c>
-      <c r="J3" s="3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="3">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
         <v>6</v>
       </c>
-      <c r="L3" s="3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3">
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="O3">
         <v>16</v>
       </c>
     </row>
@@ -1673,22 +1685,10 @@
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="O4">
         <v>1</v>
       </c>
     </row>
@@ -1696,22 +1696,10 @@
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>7</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3">
+      <c r="O5">
         <v>7</v>
       </c>
     </row>
@@ -1719,22 +1707,10 @@
       <c r="A6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3">
-        <v>1</v>
-      </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3">
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="O6">
         <v>1</v>
       </c>
     </row>
@@ -1742,22 +1718,10 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="O7">
         <v>1</v>
       </c>
     </row>
@@ -1765,22 +1729,10 @@
       <c r="A8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3">
-        <v>1</v>
-      </c>
-      <c r="O8" s="3">
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
         <v>1</v>
       </c>
     </row>
@@ -1788,321 +1740,346 @@
       <c r="A9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>7</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>2</v>
       </c>
-      <c r="E9" s="3">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3">
-        <v>1</v>
-      </c>
-      <c r="H9" s="3">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
         <v>2</v>
       </c>
-      <c r="I9" s="3">
-        <v>1</v>
-      </c>
-      <c r="J9" s="3">
-        <v>1</v>
-      </c>
-      <c r="K9" s="3">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
         <v>6</v>
       </c>
-      <c r="L9" s="3">
-        <v>1</v>
-      </c>
-      <c r="M9" s="3">
-        <v>1</v>
-      </c>
-      <c r="N9" s="3">
-        <v>1</v>
-      </c>
-      <c r="O9" s="3">
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <f>GETPIVOTDATA("Ref.",$A$1,"Description","capacitor, 1µF")</f>
         <v>2</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="5">
         <v>98</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <f>B14+C14</f>
         <v>100</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4">
+        <v>5</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <f>SUM(F3:L3)</f>
         <v>13</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="5">
         <v>87</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <f t="shared" ref="D15:D20" si="0">B15+C15</f>
         <v>100</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6" t="s">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="str">
+      <c r="A16" s="4" t="str">
         <f>A4</f>
         <v>BC547B</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <f>GETPIVOTDATA("Ref.",$A$1,"Part No.","BC547B")</f>
         <v>1</v>
       </c>
-      <c r="C16" s="5">
-        <v>1</v>
-      </c>
-      <c r="D16" s="5">
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>0.36099999999999999</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <f>D16*E16</f>
         <v>0.72199999999999998</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="G16" s="4">
+        <v>2</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="str">
+      <c r="A17" s="4" t="str">
         <f>A5</f>
         <v>LM741</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <f>GETPIVOTDATA("Ref.",$A$1,"Part No.","LM741")</f>
         <v>7</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>3</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>0.54200000000000004</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <f>D17*E17</f>
         <v>5.42</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="12">
+        <v>10</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="str">
+      <c r="A18" s="4" t="str">
         <f>A6</f>
         <v>TO126 Heatsink</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <f>GETPIVOTDATA("Ref.",$A$1,"Part No.","TO126 Heatsink")</f>
         <v>1</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>0</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>5.64</v>
       </c>
-      <c r="F18" s="5">
-        <f t="shared" ref="F18:F20" si="1">D18*E18</f>
+      <c r="F18" s="4">
+        <f>D18*E18</f>
         <v>5.64</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="12">
+        <v>1</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="str">
+      <c r="A19" s="4" t="str">
         <f>A7</f>
         <v>BD135</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <f>GETPIVOTDATA("Ref.",$A$1,"Part No.","BD135")</f>
         <v>1</v>
       </c>
-      <c r="C19" s="5">
-        <v>1</v>
-      </c>
-      <c r="D19" s="5">
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>1.05</v>
       </c>
-      <c r="F19" s="5">
-        <f t="shared" si="1"/>
+      <c r="F19" s="4">
+        <f>D19*E19</f>
         <v>2.1</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="12">
+        <v>2</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="str">
+      <c r="A20" s="4" t="str">
         <f>A8</f>
         <v>TO222 Heatsink*</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <f>GETPIVOTDATA("Ref.",$A$1,"Part No.","TO222 Heatsink*")</f>
         <v>1</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>0</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>0.9</v>
       </c>
-      <c r="F20" s="5">
-        <f t="shared" si="1"/>
+      <c r="F20" s="4">
+        <f>D20*E20</f>
         <v>0.9</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="12">
+        <v>1</v>
+      </c>
+      <c r="H20" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="10"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="11">
         <f>SUM(F14:F20)</f>
         <v>14.782</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="13"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="11">
         <v>20</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="11">
         <f>B22+B21</f>
         <v>34.781999999999996</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="B23:F23"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
   </mergeCells>
+  <conditionalFormatting sqref="G14:G20">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>G14&gt;=D14</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>